<commit_message>
Tables changed to test possible conflict with multiple loadbuilders
</commit_message>
<xml_diff>
--- a/LoadBuilding/Builder_tests/Models_and_trailers.xlsx
+++ b/LoadBuilding/Builder_tests/Models_and_trailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/Desktop/Optimus/Optimus/LoadBuilding/Builder_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FC5F39-F161-034F-B0B1-0B2F2538EF2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBC1744-E659-8D4D-A00D-7CE158AB2C15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
   <si>
     <t>VT</t>
   </si>
@@ -116,15 +116,25 @@
   </si>
   <si>
     <t>PLANT_FROM</t>
+  </si>
+  <si>
+    <t>Juarez 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -297,11 +307,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -309,16 +319,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,9 +361,7 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
+        <right/>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -393,206 +407,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -613,7 +427,9 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -902,6 +718,206 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -916,36 +932,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AD9C9D7-B776-ED48-B1A0-120D1F249EB0}" name="Models" displayName="Models" ref="A1:I17" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AD9C9D7-B776-ED48-B1A0-120D1F249EB0}" name="Models" displayName="Models" ref="A1:I17" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="A1:I17" xr:uid="{B8BD2856-03ED-B94A-BE6F-6AC067A0FA50}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5B513D7F-ADBF-2E40-A83E-AA4CDC204E06}" name="QTY" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{A8B53A9E-41C8-EA4D-8035-F9BAC85EC3EF}" name="MODEL" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{C3347BE8-E6A0-4D47-8821-34B345098848}" name="PLANT_TO" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{C4E41E7A-3A69-6A4B-B572-7B96B518B1E8}" name="LENGTH" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{7F303A2D-67E2-4249-A7E8-D6CD11CACCB0}" name="WIDTH" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{5066A8A8-3518-394C-93EA-9478573EC405}" name="HEIGHT" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{020412A2-1252-4745-AF71-6A6904F5FF1D}" name="NBR_PER_CRATE" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{6B2A8BB6-0232-5B40-B66D-72F1F14F3936}" name="STACK_LIMIT" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{E55352C4-DD59-7A4E-83E2-49BCD619B27B}" name="OVERHANG" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{5B513D7F-ADBF-2E40-A83E-AA4CDC204E06}" name="QTY" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{A8B53A9E-41C8-EA4D-8035-F9BAC85EC3EF}" name="MODEL" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{C3347BE8-E6A0-4D47-8821-34B345098848}" name="PLANT_TO" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{C4E41E7A-3A69-6A4B-B572-7B96B518B1E8}" name="LENGTH" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{7F303A2D-67E2-4249-A7E8-D6CD11CACCB0}" name="WIDTH" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{5066A8A8-3518-394C-93EA-9478573EC405}" name="HEIGHT" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{020412A2-1252-4745-AF71-6A6904F5FF1D}" name="NBR_PER_CRATE" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{6B2A8BB6-0232-5B40-B66D-72F1F14F3936}" name="STACK_LIMIT" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{E55352C4-DD59-7A4E-83E2-49BCD619B27B}" name="OVERHANG" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{145FC4D2-31CA-414A-8AD0-FAA4ED2BE800}" name="Trailers" displayName="Trailers" ref="K1:S4" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
-  <autoFilter ref="K1:S4" xr:uid="{2BC46E84-7004-454B-AC24-82F3AC8719DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{145FC4D2-31CA-414A-8AD0-FAA4ED2BE800}" name="Trailers" displayName="Trailers" ref="K1:S6" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="K1:S6" xr:uid="{2BC46E84-7004-454B-AC24-82F3AC8719DC}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{6D619528-DB4C-F44E-BE71-C53A8B5529B9}" name="QTY" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{47862604-F4CB-4540-A806-5E9BBF8F1590}" name="CATEGORY" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{77470888-3E80-154D-9247-EA8794E6DA2E}" name="PLANT_FROM" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{03667014-F4D1-B54D-B25D-8762F7F0F877}" name="PLANT_TO" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{05A2C741-6F5C-BE44-8354-1F5FF4E19FB4}" name="LENGTH" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{68A919E0-EEEC-BF4A-BB33-267B830FCAF9}" name="WIDTH" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{350D4D62-FCCE-8249-81D2-AAFCECDE2BA7}" name="HEIGHT" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{79D2C0A2-5FCC-A84E-9695-55394019DC2F}" name="OVERHANG" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{0601ABE4-24E5-6A46-AC1E-3169A568CFB8}" name="PRIORITY_RANK" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{6D619528-DB4C-F44E-BE71-C53A8B5529B9}" name="QTY" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{47862604-F4CB-4540-A806-5E9BBF8F1590}" name="CATEGORY" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{77470888-3E80-154D-9247-EA8794E6DA2E}" name="PLANT_FROM" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{03667014-F4D1-B54D-B25D-8762F7F0F877}" name="PLANT_TO" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{05A2C741-6F5C-BE44-8354-1F5FF4E19FB4}" name="LENGTH" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{68A919E0-EEEC-BF4A-BB33-267B830FCAF9}" name="WIDTH" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{350D4D62-FCCE-8249-81D2-AAFCECDE2BA7}" name="HEIGHT" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{79D2C0A2-5FCC-A84E-9695-55394019DC2F}" name="OVERHANG" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{0601ABE4-24E5-6A46-AC1E-3169A568CFB8}" name="PRIORITY_RANK" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1239,7 +1255,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1479,15 +1495,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1">
         <v>118</v>
@@ -1507,8 +1523,35 @@
       <c r="I5" s="5">
         <v>1</v>
       </c>
+      <c r="K5" s="21">
+        <v>10</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="22">
+        <v>576</v>
+      </c>
+      <c r="P5" s="22">
+        <v>102</v>
+      </c>
+      <c r="Q5" s="22">
+        <v>120</v>
+      </c>
+      <c r="R5" s="22">
+        <v>1</v>
+      </c>
+      <c r="S5" s="23">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>0</v>
       </c>
@@ -1534,6 +1577,33 @@
         <v>2</v>
       </c>
       <c r="I6" s="5">
+        <v>1</v>
+      </c>
+      <c r="K6" s="24">
+        <v>2</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="25">
+        <v>636</v>
+      </c>
+      <c r="P6" s="25">
+        <v>102</v>
+      </c>
+      <c r="Q6" s="25">
+        <v>120</v>
+      </c>
+      <c r="R6" s="25">
+        <v>0</v>
+      </c>
+      <c r="S6" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1626,7 +1696,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
@@ -1771,13 +1841,13 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1">
         <v>126</v>

</xml_diff>

<commit_message>
New test results with code fixed
</commit_message>
<xml_diff>
--- a/LoadBuilding/Builder_tests/Models_and_trailers.xlsx
+++ b/LoadBuilding/Builder_tests/Models_and_trailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/Desktop/Optimus/Optimus/LoadBuilding/Builder_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBC1744-E659-8D4D-A00D-7CE158AB2C15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F948FE7-C5CB-AC42-BDC6-9FF05E6A54C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1255,7 +1255,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Test files adapted to test stack completion
</commit_message>
<xml_diff>
--- a/LoadBuilding/Builder_tests/Models_and_trailers.xlsx
+++ b/LoadBuilding/Builder_tests/Models_and_trailers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/Desktop/Optimus/Optimus/LoadBuilding/Builder_tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\LoadAutomation\Optimus\LoadBuilding\Builder_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F948FE7-C5CB-AC42-BDC6-9FF05E6A54C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9661B4-8B39-46B3-9927-8FE02363DFDF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P2P Juarez to El Paso" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>VT</t>
   </si>
@@ -106,49 +106,19 @@
     <t>CATEGORY</t>
   </si>
   <si>
-    <t>Juarez</t>
-  </si>
-  <si>
-    <t>El Paso</t>
-  </si>
-  <si>
-    <t>PLANT_TO</t>
-  </si>
-  <si>
-    <t>PLANT_FROM</t>
-  </si>
-  <si>
-    <t>Juarez 2</t>
+    <t>CRATE_TYPE</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -307,11 +277,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -319,27 +288,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="25">
     <dxf>
       <font>
         <b val="0"/>
@@ -560,74 +525,6 @@
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color auto="1"/>
@@ -719,23 +616,24 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -748,8 +646,6 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -932,31 +828,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AD9C9D7-B776-ED48-B1A0-120D1F249EB0}" name="Models" displayName="Models" ref="A1:I17" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AD9C9D7-B776-ED48-B1A0-120D1F249EB0}" name="Models" displayName="Models" ref="A1:I17" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="A1:I17" xr:uid="{B8BD2856-03ED-B94A-BE6F-6AC067A0FA50}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5B513D7F-ADBF-2E40-A83E-AA4CDC204E06}" name="QTY" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{A8B53A9E-41C8-EA4D-8035-F9BAC85EC3EF}" name="MODEL" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{C3347BE8-E6A0-4D47-8821-34B345098848}" name="PLANT_TO" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{C4E41E7A-3A69-6A4B-B572-7B96B518B1E8}" name="LENGTH" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{7F303A2D-67E2-4249-A7E8-D6CD11CACCB0}" name="WIDTH" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{5066A8A8-3518-394C-93EA-9478573EC405}" name="HEIGHT" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{020412A2-1252-4745-AF71-6A6904F5FF1D}" name="NBR_PER_CRATE" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{6B2A8BB6-0232-5B40-B66D-72F1F14F3936}" name="STACK_LIMIT" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{E55352C4-DD59-7A4E-83E2-49BCD619B27B}" name="OVERHANG" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{5B513D7F-ADBF-2E40-A83E-AA4CDC204E06}" name="QTY" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{A8B53A9E-41C8-EA4D-8035-F9BAC85EC3EF}" name="MODEL" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{C4E41E7A-3A69-6A4B-B572-7B96B518B1E8}" name="LENGTH" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{7F303A2D-67E2-4249-A7E8-D6CD11CACCB0}" name="WIDTH" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{5066A8A8-3518-394C-93EA-9478573EC405}" name="HEIGHT" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{020412A2-1252-4745-AF71-6A6904F5FF1D}" name="NBR_PER_CRATE" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{6B2A8BB6-0232-5B40-B66D-72F1F14F3936}" name="STACK_LIMIT" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{E55352C4-DD59-7A4E-83E2-49BCD619B27B}" name="OVERHANG" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{7B63EFBD-5C17-45AD-BEEE-B41125887685}" name="CRATE_TYPE" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{145FC4D2-31CA-414A-8AD0-FAA4ED2BE800}" name="Trailers" displayName="Trailers" ref="K1:S6" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="K1:S6" xr:uid="{2BC46E84-7004-454B-AC24-82F3AC8719DC}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{6D619528-DB4C-F44E-BE71-C53A8B5529B9}" name="QTY" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{47862604-F4CB-4540-A806-5E9BBF8F1590}" name="CATEGORY" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{77470888-3E80-154D-9247-EA8794E6DA2E}" name="PLANT_FROM" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{03667014-F4D1-B54D-B25D-8762F7F0F877}" name="PLANT_TO" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{145FC4D2-31CA-414A-8AD0-FAA4ED2BE800}" name="Trailers" displayName="Trailers" ref="K1:Q3" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="K1:Q3" xr:uid="{2BC46E84-7004-454B-AC24-82F3AC8719DC}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{6D619528-DB4C-F44E-BE71-C53A8B5529B9}" name="QTY" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{47862604-F4CB-4540-A806-5E9BBF8F1590}" name="CATEGORY" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{05A2C741-6F5C-BE44-8354-1F5FF4E19FB4}" name="LENGTH" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{68A919E0-EEEC-BF4A-BB33-267B830FCAF9}" name="WIDTH" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{350D4D62-FCCE-8249-81D2-AAFCECDE2BA7}" name="HEIGHT" dataDxfId="2"/>
@@ -1252,678 +1146,578 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318A87B4-B040-8645-BE5D-1CAEBC114D14}">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" customWidth="1"/>
-    <col min="17" max="17" width="17" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="9" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="G1" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="H1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="I1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>23</v>
       </c>
+      <c r="N1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>25</v>
+      </c>
       <c r="P1" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="Q1" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1">
+        <v>90</v>
+      </c>
+      <c r="D2" s="1">
+        <v>51</v>
+      </c>
+      <c r="E2" s="1">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="1">
-        <v>90</v>
-      </c>
-      <c r="E2" s="1">
-        <v>51</v>
-      </c>
-      <c r="F2" s="1">
-        <v>49</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1">
-        <v>2</v>
-      </c>
-      <c r="I2" s="5">
-        <v>1</v>
-      </c>
-      <c r="K2" s="11">
+      <c r="K2" s="10">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="20" t="s">
+      <c r="M2" s="2">
+        <v>576</v>
+      </c>
+      <c r="N2" s="2">
+        <v>102</v>
+      </c>
+      <c r="O2" s="2">
+        <v>105</v>
+      </c>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>98</v>
+      </c>
+      <c r="D3" s="1">
+        <v>51</v>
+      </c>
+      <c r="E3" s="1">
+        <v>49</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="2">
-        <v>576</v>
-      </c>
-      <c r="P2" s="2">
-        <v>102</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>120</v>
-      </c>
-      <c r="R2" s="2">
-        <v>1</v>
-      </c>
-      <c r="S2" s="12">
+      <c r="K3" s="18">
+        <v>0</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="16">
+        <v>628</v>
+      </c>
+      <c r="N3" s="16">
+        <v>98</v>
+      </c>
+      <c r="O3" s="16">
+        <v>105</v>
+      </c>
+      <c r="P3" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="1">
-        <v>98</v>
-      </c>
-      <c r="E3" s="1">
-        <v>51</v>
-      </c>
-      <c r="F3" s="1">
-        <v>49</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>2</v>
-      </c>
-      <c r="I3" s="5">
-        <v>1</v>
-      </c>
-      <c r="K3" s="11">
-        <v>2</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="2">
-        <v>636</v>
-      </c>
-      <c r="P3" s="2">
-        <v>102</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>120</v>
-      </c>
-      <c r="R3" s="2">
-        <v>0</v>
-      </c>
-      <c r="S3" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="1">
+        <v>98</v>
+      </c>
+      <c r="D4" s="1">
+        <v>56</v>
+      </c>
+      <c r="E4" s="1">
+        <v>49</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="1">
-        <v>98</v>
-      </c>
-      <c r="E4" s="1">
-        <v>56</v>
-      </c>
-      <c r="F4" s="1">
-        <v>49</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
-        <v>2</v>
-      </c>
-      <c r="I4" s="5">
-        <v>1</v>
-      </c>
-      <c r="K4" s="19">
-        <v>0</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="17">
-        <v>628</v>
-      </c>
-      <c r="P4" s="17">
-        <v>98</v>
-      </c>
-      <c r="Q4" s="17">
-        <v>120</v>
-      </c>
-      <c r="R4" s="17">
-        <v>0</v>
-      </c>
-      <c r="S4" s="18">
-        <v>1</v>
-      </c>
     </row>
-    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>32</v>
+      <c r="C5" s="1">
+        <v>118</v>
       </c>
       <c r="D5" s="1">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="E5" s="1">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F5" s="1">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
         <v>2</v>
       </c>
-      <c r="I5" s="5">
-        <v>1</v>
-      </c>
-      <c r="K5" s="21">
-        <v>10</v>
-      </c>
-      <c r="L5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="22">
-        <v>576</v>
-      </c>
-      <c r="P5" s="22">
-        <v>102</v>
-      </c>
-      <c r="Q5" s="22">
-        <v>120</v>
-      </c>
-      <c r="R5" s="22">
-        <v>1</v>
-      </c>
-      <c r="S5" s="23">
-        <v>1</v>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="1">
+        <v>90</v>
+      </c>
+      <c r="D6" s="1">
+        <v>56</v>
+      </c>
+      <c r="E6" s="1">
+        <v>49</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="1">
-        <v>90</v>
-      </c>
-      <c r="E6" s="1">
-        <v>56</v>
-      </c>
-      <c r="F6" s="1">
-        <v>49</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
-        <v>2</v>
-      </c>
-      <c r="I6" s="5">
-        <v>1</v>
-      </c>
-      <c r="K6" s="24">
-        <v>2</v>
-      </c>
-      <c r="L6" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="N6" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="O6" s="25">
-        <v>636</v>
-      </c>
-      <c r="P6" s="25">
-        <v>102</v>
-      </c>
-      <c r="Q6" s="25">
-        <v>120</v>
-      </c>
-      <c r="R6" s="25">
-        <v>0</v>
-      </c>
-      <c r="S6" s="26">
-        <v>1</v>
-      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="1">
+        <v>126</v>
+      </c>
+      <c r="D7" s="1">
+        <v>56</v>
+      </c>
+      <c r="E7" s="1">
+        <v>49</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="1">
-        <v>126</v>
-      </c>
-      <c r="E7" s="1">
-        <v>56</v>
-      </c>
-      <c r="F7" s="1">
-        <v>49</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>2</v>
-      </c>
-      <c r="I7" s="5">
-        <v>1</v>
-      </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="1">
+        <v>126</v>
+      </c>
+      <c r="D8" s="1">
+        <v>68</v>
+      </c>
+      <c r="E8" s="1">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="1">
-        <v>126</v>
-      </c>
-      <c r="E8" s="1">
-        <v>68</v>
-      </c>
-      <c r="F8" s="1">
-        <v>49</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
-        <v>2</v>
-      </c>
-      <c r="I8" s="5">
-        <v>1</v>
-      </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="1">
+        <v>126</v>
+      </c>
+      <c r="D9" s="1">
+        <v>75</v>
+      </c>
+      <c r="E9" s="1">
+        <v>49</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1">
-        <v>126</v>
-      </c>
-      <c r="E9" s="1">
-        <v>75</v>
-      </c>
-      <c r="F9" s="1">
-        <v>49</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1">
-        <v>2</v>
-      </c>
-      <c r="I9" s="5">
-        <v>1</v>
-      </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="1">
+        <v>132</v>
+      </c>
+      <c r="D10" s="1">
+        <v>75</v>
+      </c>
+      <c r="E10" s="1">
+        <v>49</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
+      <c r="I10" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1">
-        <v>132</v>
-      </c>
-      <c r="E10" s="1">
-        <v>75</v>
-      </c>
-      <c r="F10" s="1">
-        <v>49</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1">
-        <v>2</v>
-      </c>
-      <c r="I10" s="5">
-        <v>1</v>
-      </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="1">
+        <v>138</v>
+      </c>
+      <c r="D11" s="1">
+        <v>80</v>
+      </c>
+      <c r="E11" s="1">
+        <v>51</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="1">
-        <v>138</v>
-      </c>
-      <c r="E11" s="1">
-        <v>80</v>
-      </c>
-      <c r="F11" s="1">
-        <v>51</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
-        <v>2</v>
-      </c>
-      <c r="I11" s="5">
-        <v>1</v>
-      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="1">
+        <v>156</v>
+      </c>
+      <c r="D12" s="1">
+        <v>75</v>
+      </c>
+      <c r="E12" s="1">
+        <v>49</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="1">
-        <v>156</v>
-      </c>
-      <c r="E12" s="1">
-        <v>75</v>
-      </c>
-      <c r="F12" s="1">
-        <v>49</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1">
-        <v>2</v>
-      </c>
-      <c r="I12" s="5">
-        <v>1</v>
-      </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="1">
+        <v>172</v>
+      </c>
+      <c r="D13" s="1">
+        <v>82</v>
+      </c>
+      <c r="E13" s="1">
+        <v>52</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2</v>
+      </c>
+      <c r="H13" s="4">
+        <v>1</v>
+      </c>
+      <c r="I13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="1">
-        <v>172</v>
-      </c>
-      <c r="E13" s="1">
-        <v>82</v>
-      </c>
-      <c r="F13" s="1">
-        <v>52</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1">
-        <v>2</v>
-      </c>
-      <c r="I13" s="5">
-        <v>1</v>
-      </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="1">
+        <v>162</v>
+      </c>
+      <c r="D14" s="1">
+        <v>75</v>
+      </c>
+      <c r="E14" s="1">
+        <v>51</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>2</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="1">
-        <v>162</v>
-      </c>
-      <c r="E14" s="1">
-        <v>75</v>
-      </c>
-      <c r="F14" s="1">
-        <v>51</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1">
-        <v>2</v>
-      </c>
-      <c r="I14" s="5">
-        <v>1</v>
-      </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>32</v>
+      <c r="C15" s="1">
+        <v>126</v>
       </c>
       <c r="D15" s="1">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="E15" s="1">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F15" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1">
         <v>1</v>
       </c>
-      <c r="H15" s="1">
-        <v>1</v>
-      </c>
-      <c r="I15" s="5">
+      <c r="H15" s="4">
         <v>0</v>
       </c>
+      <c r="I15" s="19" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="1">
+        <v>159</v>
+      </c>
+      <c r="D16" s="1">
+        <v>75</v>
+      </c>
+      <c r="E16" s="1">
+        <v>50</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="1">
-        <v>159</v>
-      </c>
-      <c r="E16" s="1">
-        <v>75</v>
-      </c>
-      <c r="F16" s="1">
-        <v>50</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1">
-        <v>1</v>
-      </c>
-      <c r="I16" s="5">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="B17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="8">
+        <v>98</v>
+      </c>
+      <c r="D17" s="8">
+        <v>90</v>
+      </c>
+      <c r="E17" s="8">
+        <v>35</v>
+      </c>
+      <c r="F17" s="8">
+        <v>2</v>
+      </c>
+      <c r="G17" s="8">
+        <v>3</v>
+      </c>
+      <c r="H17" s="9">
         <v>0</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="I17" s="19" t="s">
         <v>29</v>
-      </c>
-      <c r="D17" s="9">
-        <v>98</v>
-      </c>
-      <c r="E17" s="9">
-        <v>90</v>
-      </c>
-      <c r="F17" s="9">
-        <v>35</v>
-      </c>
-      <c r="G17" s="9">
-        <v>2</v>
-      </c>
-      <c r="H17" s="9">
-        <v>3</v>
-      </c>
-      <c r="I17" s="10">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Qty adapted to test attribute patching_activated of LoadBuilder class
</commit_message>
<xml_diff>
--- a/LoadBuilding/Builder_tests/Models_and_trailers.xlsx
+++ b/LoadBuilding/Builder_tests/Models_and_trailers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\LoadAutomation\Optimus\LoadBuilding\Builder_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9661B4-8B39-46B3-9927-8FE02363DFDF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561DD7C0-E567-4D39-9417-240C64940001}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35880" yWindow="2760" windowWidth="14250" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P2P Juarez to El Paso" sheetId="2" r:id="rId1"/>
@@ -1149,7 +1149,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Models in file updated
</commit_message>
<xml_diff>
--- a/LoadBuilding/Builder_tests/Models_and_trailers.xlsx
+++ b/LoadBuilding/Builder_tests/Models_and_trailers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\LoadAutomation\Optimus\LoadBuilding\Builder_tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raymoni.BRP\Desktop\untitled1\Optimus\LoadBuilding\Builder_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561DD7C0-E567-4D39-9417-240C64940001}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F398C0A-89E4-474E-8460-6BB7318AB90C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35880" yWindow="2760" windowWidth="14250" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P2P Juarez to El Paso" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>VT</t>
   </si>
@@ -1146,13 +1146,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318A87B4-B040-8645-BE5D-1CAEBC114D14}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" customWidth="1"/>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1228,7 +1228,7 @@
         <v>51</v>
       </c>
       <c r="E2" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -1243,7 +1243,7 @@
         <v>29</v>
       </c>
       <c r="K2" s="10">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>21</v>
@@ -1266,19 +1266,19 @@
     </row>
     <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3" s="1">
         <v>51</v>
       </c>
       <c r="E3" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -1299,7 +1299,7 @@
         <v>16</v>
       </c>
       <c r="M3" s="16">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="N3" s="16">
         <v>98</v>
@@ -1316,19 +1316,19 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D4" s="1">
         <v>56</v>
       </c>
       <c r="E4" s="1">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -1374,19 +1374,19 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D6" s="1">
         <v>56</v>
       </c>
       <c r="E6" s="1">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
@@ -1403,7 +1403,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -1415,7 +1415,7 @@
         <v>56</v>
       </c>
       <c r="E7" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -1545,6 +1545,12 @@
       <c r="I11" s="19" t="s">
         <v>29</v>
       </c>
+      <c r="L11">
+        <v>3</v>
+      </c>
+      <c r="M11" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -1574,6 +1580,12 @@
       <c r="I12" s="19" t="s">
         <v>29</v>
       </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -1603,6 +1615,12 @@
       <c r="I13" s="19" t="s">
         <v>29</v>
       </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -1632,6 +1650,12 @@
       <c r="I14" s="19" t="s">
         <v>29</v>
       </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -1661,6 +1685,12 @@
       <c r="I15" s="19" t="s">
         <v>29</v>
       </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -1690,8 +1720,14 @@
       <c r="I16" s="19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>0</v>
       </c>
@@ -1718,6 +1754,68 @@
       </c>
       <c r="I17" s="19" t="s">
         <v>29</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>